<commit_message>
Added mode baseload controller
</commit_message>
<xml_diff>
--- a/ems_dict_v06.xlsx
+++ b/ems_dict_v06.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.101.142\admin\projects\python\ems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DB59EB-E184-4863-91A9-45E11A91C8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596DFC5C-1A6B-4BA4-9A64-9A265B9DC3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="7" xr2:uid="{75D214A9-D7AF-49D5-B041-EC14400D16F0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{75D214A9-D7AF-49D5-B041-EC14400D16F0}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_REGISTER_LIST" sheetId="29" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7979" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7991" uniqueCount="1069">
   <si>
     <t>DSMR</t>
   </si>
@@ -3186,15 +3186,9 @@
     <t>"u"</t>
   </si>
   <si>
-    <t>"value"</t>
-  </si>
-  <si>
     <t>"W"</t>
   </si>
   <si>
-    <t>"m3"</t>
-  </si>
-  <si>
     <t>HOME_PWR_TOT</t>
   </si>
   <si>
@@ -3207,18 +3201,9 @@
     <t>HOME_PWR_L3</t>
   </si>
   <si>
-    <t>HOME_GAS_TIME_STAMP</t>
-  </si>
-  <si>
-    <t>HOME_GAS_VOLUME</t>
-  </si>
-  <si>
     <t>""</t>
   </si>
   <si>
-    <t xml:space="preserve"> ,</t>
-  </si>
-  <si>
     <t>HOME_PWR_TIME_STAMP</t>
   </si>
   <si>
@@ -3237,10 +3222,46 @@
     <t>Power phase 3 (signed, consume is positive)</t>
   </si>
   <si>
-    <t>Timestamp gas</t>
-  </si>
-  <si>
-    <t>Volume (m3)</t>
+    <t>init_value</t>
+  </si>
+  <si>
+    <t>HOME_PWR_CONS</t>
+  </si>
+  <si>
+    <t>HOME_PWR_PROD</t>
+  </si>
+  <si>
+    <t>"s"</t>
+  </si>
+  <si>
+    <t>Power consumed total (unsigned always positive)</t>
+  </si>
+  <si>
+    <t>Power produced total (unsigned always positive)</t>
+  </si>
+  <si>
+    <t># --- HOME_FIELD_INDEX index for HOME POWER values</t>
+  </si>
+  <si>
+    <t>IDXH_NAME</t>
+  </si>
+  <si>
+    <t>IDXH_SIGN</t>
+  </si>
+  <si>
+    <t>IDXH_HVAL</t>
+  </si>
+  <si>
+    <t>IDXH_UNIT</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>dagen</t>
   </si>
 </sst>
 </file>
@@ -3397,7 +3418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3517,6 +3538,7 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -28058,10 +28080,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28056F46-B4A9-4770-A5AA-63501C9B5AD4}">
-  <dimension ref="A1:AA79"/>
+  <dimension ref="A1:AC79"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Z55" sqref="Z55"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33282,7 +33304,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A65" s="29" t="s">
         <v>684</v>
       </c>
@@ -33365,7 +33387,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
         <v>684</v>
       </c>
@@ -33448,7 +33470,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A67" s="30" t="s">
         <v>684</v>
       </c>
@@ -33531,7 +33553,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A68" s="29" t="s">
         <v>684</v>
       </c>
@@ -33614,7 +33636,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A69" s="29" t="s">
         <v>684</v>
       </c>
@@ -33697,7 +33719,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A70" s="30" t="s">
         <v>684</v>
       </c>
@@ -33780,7 +33802,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A71" s="29" t="s">
         <v>684</v>
       </c>
@@ -33863,7 +33885,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
         <v>684</v>
       </c>
@@ -33945,8 +33967,9 @@
       <c r="AA72" s="7" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC72" s="55"/>
+    </row>
+    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
         <v>684</v>
       </c>
@@ -34029,7 +34052,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A74" s="29" t="s">
         <v>684</v>
       </c>
@@ -34112,19 +34135,19 @@
         <v>760</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F79" s="1"/>
     </row>
   </sheetData>
@@ -34372,7 +34395,7 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:V51"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -37449,10 +37472,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71E96B6-E01B-48D5-AC3C-7C59A84F3179}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:R7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37463,21 +37486,22 @@
     <col min="4" max="4" width="1.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="1.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" customWidth="1"/>
     <col min="10" max="10" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.85546875" customWidth="1"/>
+    <col min="18" max="18" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>688</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>1054</v>
+        <v>1049</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>685</v>
@@ -37492,19 +37516,19 @@
         <v>686</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>1043</v>
+        <v>1055</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>686</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
       <c r="J1" s="18" t="s">
         <v>903</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>1054</v>
+        <v>1049</v>
       </c>
       <c r="N1" s="54" t="s">
         <v>121</v>
@@ -37517,15 +37541,20 @@
         <v>690</v>
       </c>
       <c r="R1" s="18" t="s">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1050</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>1061</v>
+      </c>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>688</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>1046</v>
+        <v>1056</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>685</v>
@@ -37540,19 +37569,19 @@
         <v>686</v>
       </c>
       <c r="G2" s="18" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>686</v>
+      </c>
+      <c r="I2" s="18" t="s">
         <v>1043</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>686</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>1044</v>
       </c>
       <c r="J2" s="18" t="s">
         <v>903</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>1046</v>
+        <v>1056</v>
       </c>
       <c r="N2" s="54" t="s">
         <v>121</v>
@@ -37565,15 +37594,24 @@
         <v>690</v>
       </c>
       <c r="R2" s="18" t="s">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1059</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>1062</v>
+      </c>
+      <c r="U2" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="V2" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>688</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>1047</v>
+        <v>1057</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>685</v>
@@ -37588,19 +37626,19 @@
         <v>686</v>
       </c>
       <c r="G3" s="18" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>686</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>1043</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>686</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>1044</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>903</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>1047</v>
+        <v>1057</v>
       </c>
       <c r="N3" s="54" t="s">
         <v>121</v>
@@ -37613,15 +37651,24 @@
         <v>690</v>
       </c>
       <c r="R3" s="18" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1060</v>
+      </c>
+      <c r="T3" s="18" t="s">
+        <v>1063</v>
+      </c>
+      <c r="U3" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="V3" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>688</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>685</v>
@@ -37630,25 +37677,25 @@
         <v>686</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>1042</v>
+        <v>1058</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>686</v>
       </c>
       <c r="G4" s="18" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>686</v>
+      </c>
+      <c r="I4" s="18" t="s">
         <v>1043</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>686</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>1044</v>
       </c>
       <c r="J4" s="18" t="s">
         <v>903</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="N4" s="54" t="s">
         <v>121</v>
@@ -37661,15 +37708,24 @@
         <v>690</v>
       </c>
       <c r="R4" s="18" t="s">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1052</v>
+      </c>
+      <c r="T4" s="18" t="s">
+        <v>1064</v>
+      </c>
+      <c r="U4" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="V4" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>688</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>685</v>
@@ -37678,25 +37734,25 @@
         <v>686</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>1042</v>
+        <v>1058</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>686</v>
       </c>
       <c r="G5" s="18" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>686</v>
+      </c>
+      <c r="I5" s="18" t="s">
         <v>1043</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>686</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>1044</v>
       </c>
       <c r="J5" s="18" t="s">
         <v>903</v>
       </c>
       <c r="M5" s="18" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
       <c r="N5" s="54" t="s">
         <v>121</v>
@@ -37709,15 +37765,24 @@
         <v>690</v>
       </c>
       <c r="R5" s="18" t="s">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1051</v>
+      </c>
+      <c r="T5" s="18" t="s">
+        <v>1065</v>
+      </c>
+      <c r="U5" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="V5" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>688</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>685</v>
@@ -37726,25 +37791,25 @@
         <v>686</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>1041</v>
+        <v>1058</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>686</v>
       </c>
       <c r="G6" s="18" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>686</v>
+      </c>
+      <c r="I6" s="18" t="s">
         <v>1043</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>1053</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>1052</v>
       </c>
       <c r="J6" s="18" t="s">
         <v>903</v>
       </c>
       <c r="M6" s="18" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
       <c r="N6" s="54" t="s">
         <v>121</v>
@@ -37757,15 +37822,15 @@
         <v>690</v>
       </c>
       <c r="R6" s="18" t="s">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>688</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>685</v>
@@ -37774,25 +37839,25 @@
         <v>686</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>1042</v>
+        <v>1058</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>686</v>
       </c>
       <c r="G7" s="18" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>686</v>
+      </c>
+      <c r="I7" s="18" t="s">
         <v>1043</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>686</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>1045</v>
       </c>
       <c r="J7" s="18" t="s">
         <v>741</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="N7" s="54" t="s">
         <v>121</v>
@@ -37805,7 +37870,7 @@
         <v>690</v>
       </c>
       <c r="R7" s="18" t="s">
-        <v>1061</v>
+        <v>1054</v>
       </c>
     </row>
   </sheetData>
@@ -37816,10 +37881,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AAB428-73A0-454D-A481-34E62C5D0098}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37832,7 +37897,7 @@
     <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>688</v>
       </c>
@@ -37852,7 +37917,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>688</v>
       </c>
@@ -37872,7 +37937,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>688</v>
       </c>
@@ -37892,7 +37957,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>688</v>
       </c>
@@ -37912,7 +37977,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>688</v>
       </c>
@@ -37932,7 +37997,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>688</v>
       </c>
@@ -37952,7 +38017,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>688</v>
       </c>
@@ -37972,7 +38037,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>688</v>
       </c>
@@ -37991,8 +38056,11 @@
       <c r="F8" s="9" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>688</v>
       </c>
@@ -38011,8 +38079,15 @@
       <c r="F9" s="9" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f>J8/60</f>
+        <v>16666.666666666668</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>688</v>
       </c>
@@ -38031,8 +38106,15 @@
       <c r="F10" s="9" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f>J9/60</f>
+        <v>277.77777777777777</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>688</v>
       </c>
@@ -38051,8 +38133,15 @@
       <c r="F11" s="9" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f>J10/24</f>
+        <v>11.574074074074074</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>688</v>
       </c>
@@ -38072,7 +38161,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>688</v>
       </c>
@@ -38092,7 +38181,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>688</v>
       </c>
@@ -38112,7 +38201,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>688</v>
       </c>
@@ -38132,7 +38221,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>688</v>
       </c>

</xml_diff>